<commit_message>
Uniques, pipelines regr, class revisiting
</commit_message>
<xml_diff>
--- a/data/Influencers_OLS.xlsx
+++ b/data/Influencers_OLS.xlsx
@@ -446,102 +446,102 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>678</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>712</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>214</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>549</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>625</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>863</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>229</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>526</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>725</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>408</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>351</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>375</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>584</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>625</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>214</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>712</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>871</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>471</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>229</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>863</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>678</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>526</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>871</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>549</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>864</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>334</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>408</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>351</t>
         </is>
       </c>
     </row>
@@ -588,13 +588,13 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>0.1508</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1508</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -640,41 +640,41 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="R3" t="n">
         <v>2.42</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0767</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -728,22 +728,22 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>5.8839</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>11.9724</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>0.0767</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>0.0767</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0767</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>0.2047</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -755,13 +755,13 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2047</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>5.8839</v>
       </c>
     </row>
     <row r="5">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1188</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -801,22 +801,22 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1.1592</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
         <v>0.1394</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.0336</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>0.1188</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0336</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>0.07489999999999999</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
@@ -828,13 +828,13 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0.07489999999999999</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>1.1592</v>
       </c>
     </row>
     <row r="6">
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0595</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5558</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0.8535</v>
@@ -883,13 +883,13 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>0.0595</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>3.156</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -901,13 +901,13 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>3.156</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>0.5558</v>
       </c>
     </row>
     <row r="7">
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0504</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -947,22 +947,22 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1512</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>4.9051</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>1.2431</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="P7" t="n">
-        <v>1.2431</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.168</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -974,13 +974,13 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>0.1512</v>
       </c>
     </row>
     <row r="8">
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2.3622</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1020,22 +1020,22 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3656</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>2.7326</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>1.2749</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>2.3622</v>
       </c>
       <c r="P8" t="n">
-        <v>1.2749</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>0.3127</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1047,13 +1047,13 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.3127</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>0.3656</v>
       </c>
     </row>
     <row r="9">
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08550000000000001</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1093,22 +1093,22 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.2541</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0.9258999999999999</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.1686</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>0.08550000000000001</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1686</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>3.4666</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1120,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>3.4666</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>0.2541</v>
       </c>
     </row>
     <row r="10">
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.1059</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1059</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -1215,64 +1215,64 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2643</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2517</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.7054</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.661</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.1762</v>
       </c>
-      <c r="E11" t="n">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.8498</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.4404</v>
+      </c>
+      <c r="T11" t="n">
         <v>0.7927999999999999</v>
       </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.8498</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="U11" t="n">
         <v>0.0126</v>
       </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.2643</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1.661</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>2.7054</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0.2517</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0</v>
-      </c>
       <c r="V11" t="n">
-        <v>0.151</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>0.4404</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1361,64 +1361,64 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2466</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.2332</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3.2821</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
         <v>0.3035</v>
       </c>
-      <c r="E13" t="n">
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2.1628</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.3035</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.1138</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.6261</v>
+      </c>
+      <c r="T13" t="n">
         <v>0.702</v>
       </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.1138</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.2466</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>2.1628</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.3035</v>
-      </c>
-      <c r="S13" t="n">
-        <v>3.2821</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0</v>
-      </c>
       <c r="U13" t="n">
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>1.2332</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0.6261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1443,40 +1443,40 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.0144</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -1519,25 +1519,25 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
         <v>0.295</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0047</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1326</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -1604,22 +1604,22 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7877</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
         <v>0.8999</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>0.0867</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>0.1326</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0867</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>0.4334</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -1631,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.4334</v>
+        <v>0</v>
       </c>
       <c r="V16" t="n">
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>0</v>
+        <v>0.7877</v>
       </c>
     </row>
     <row r="17">
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>0.3597</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>0.3597</v>
+        <v>0</v>
       </c>
       <c r="V17" t="n">
         <v>0</v>
@@ -1729,58 +1729,58 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0298</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.0944</v>
       </c>
-      <c r="H18" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.0298</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
-      </c>
       <c r="S18" t="n">
         <v>0</v>
       </c>
       <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
         <v>0.009900000000000001</v>
       </c>
-      <c r="U18" t="n">
-        <v>0</v>
-      </c>
       <c r="V18" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
         <v>0</v>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8107</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1823,13 +1823,13 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>0.3076</v>
       </c>
       <c r="M19" t="n">
         <v>0.0029</v>
       </c>
       <c r="N19" t="n">
-        <v>0.3076</v>
+        <v>0</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
@@ -1838,25 +1838,25 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>0.0259</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>0.8107</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
       </c>
       <c r="U19" t="n">
-        <v>0.0259</v>
+        <v>0</v>
       </c>
       <c r="V19" t="n">
         <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>0.06610000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1884,17 +1884,17 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.3998</v>
+      </c>
+      <c r="K20" t="n">
         <v>0.0013</v>
       </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>0.3998</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>0.0016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2018,64 +2018,64 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
+        <v>1.4986</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0117</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0391</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.4751</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>7.1605</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.4617</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.2191</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
         <v>0.0078</v>
       </c>
-      <c r="E22" t="n">
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>5.1571</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="T22" t="n">
         <v>0.1683</v>
       </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5.1571</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.4617</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.0117</v>
-      </c>
-      <c r="K22" t="n">
-        <v>1.4751</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0.2191</v>
-      </c>
-      <c r="O22" t="n">
-        <v>1.4986</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="n">
+      <c r="U22" t="n">
+        <v>1.7373</v>
+      </c>
+      <c r="V22" t="n">
         <v>0.4069</v>
       </c>
-      <c r="R22" t="n">
-        <v>7.1605</v>
-      </c>
-      <c r="S22" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="T22" t="n">
-        <v>1.7373</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" t="n">
-        <v>0.0391</v>
-      </c>
       <c r="W22" t="n">
-        <v>0.0157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.8231</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -2115,22 +2115,22 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1343</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
         <v>0.5757</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>0.0192</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>1.8231</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0192</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>0.2687</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -2142,13 +2142,13 @@
         <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>0.2687</v>
+        <v>0</v>
       </c>
       <c r="V23" t="n">
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>0.1343</v>
       </c>
     </row>
     <row r="24">
@@ -2164,64 +2164,64 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.4854</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3069</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2946</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.3069</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.8102</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
         <v>3.5846</v>
       </c>
-      <c r="E24" t="n">
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.2332</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.4297</v>
+      </c>
+      <c r="T24" t="n">
         <v>0.6875</v>
       </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.2332</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>1.4854</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0.0123</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0.8102</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0.3069</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0.2946</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>0.3069</v>
+        <v>0</v>
       </c>
       <c r="W24" t="n">
-        <v>0.4297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2276,25 +2276,25 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>0.1704</v>
       </c>
       <c r="R25" t="n">
         <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>0</v>
+        <v>0.7262999999999999</v>
       </c>
       <c r="T25" t="n">
         <v>0</v>
       </c>
       <c r="U25" t="n">
-        <v>0.1704</v>
+        <v>0</v>
       </c>
       <c r="V25" t="n">
         <v>0</v>
       </c>
       <c r="W25" t="n">
-        <v>0.7262999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2413,17 +2413,17 @@
         <v>0.06909999999999999</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>0.0395</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
       </c>
       <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
         <v>0.0395</v>
       </c>
-      <c r="Q27" t="n">
-        <v>0</v>
-      </c>
       <c r="R27" t="n">
         <v>0</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="U27" t="n">
-        <v>0.0395</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
         <v>0</v>
@@ -2465,41 +2465,41 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.948</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="R28" t="n">
         <v>0.5959</v>
       </c>
-      <c r="H28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="n">
-        <v>0.948</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="n">
-        <v>0</v>
-      </c>
       <c r="S28" t="n">
         <v>0</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="U28" t="n">
-        <v>0.0271</v>
+        <v>0</v>
       </c>
       <c r="V28" t="n">
         <v>0</v>
@@ -2559,13 +2559,13 @@
         <v>0.55</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="O29" t="n">
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
@@ -2602,56 +2602,56 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>3.0972</v>
       </c>
       <c r="E30" t="n">
+        <v>0.2099</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.4328</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.0579</v>
+      </c>
+      <c r="T30" t="n">
         <v>0.5934</v>
       </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.0145</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0.2099</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>3.0972</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="n">
-        <v>1.4328</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0</v>
-      </c>
       <c r="U30" t="n">
         <v>0</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="W30" t="n">
-        <v>0.0579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2684,55 +2684,55 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.4151</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.0511</v>
+      </c>
+      <c r="R31" t="n">
         <v>0.2917</v>
       </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="n">
-        <v>0.4151</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="n">
-        <v>0</v>
-      </c>
       <c r="S31" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="T31" t="n">
         <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>0.0511</v>
+        <v>0</v>
       </c>
       <c r="V31" t="n">
         <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2757,55 +2757,55 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.8921</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.0277</v>
+      </c>
+      <c r="R32" t="n">
         <v>0.1908</v>
       </c>
-      <c r="H32" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0.8921</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
-      </c>
       <c r="S32" t="n">
-        <v>0</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="T32" t="n">
         <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>0.0277</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
         <v>0</v>
       </c>
       <c r="W32" t="n">
-        <v>0.008200000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2845,13 +2845,13 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>0.0107</v>
       </c>
       <c r="M33" t="n">
         <v>0.0493</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0107</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
@@ -2860,25 +2860,25 @@
         <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>0.0129</v>
       </c>
       <c r="R33" t="n">
         <v>0</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>0.0278</v>
       </c>
       <c r="T33" t="n">
         <v>0</v>
       </c>
       <c r="U33" t="n">
-        <v>0.0129</v>
+        <v>0</v>
       </c>
       <c r="V33" t="n">
         <v>0</v>
       </c>
       <c r="W33" t="n">
-        <v>0.0278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2918,13 +2918,13 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>0.0182</v>
       </c>
       <c r="M34" t="n">
         <v>0.19</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0182</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
         <v>0</v>
@@ -2933,25 +2933,25 @@
         <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>0.1065</v>
       </c>
       <c r="R34" t="n">
         <v>0</v>
       </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>0.0339</v>
       </c>
       <c r="T34" t="n">
         <v>0</v>
       </c>
       <c r="U34" t="n">
-        <v>0.1065</v>
+        <v>0</v>
       </c>
       <c r="V34" t="n">
         <v>0</v>
       </c>
       <c r="W34" t="n">
-        <v>0.0339</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2967,64 +2967,64 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4.4009</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2.2016</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2.8605</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.2292</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.0044</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1.536</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
         <v>2.0539</v>
       </c>
-      <c r="E35" t="n">
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="S35" t="n">
+        <v>5.0709</v>
+      </c>
+      <c r="T35" t="n">
         <v>0.6016</v>
       </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.0044</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>4.4009</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>1.536</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="n">
-        <v>0.2292</v>
-      </c>
-      <c r="S35" t="n">
-        <v>2.8605</v>
-      </c>
-      <c r="T35" t="n">
+      <c r="U35" t="n">
         <v>0.0022</v>
       </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
       <c r="V35" t="n">
-        <v>2.2016</v>
+        <v>0</v>
       </c>
       <c r="W35" t="n">
-        <v>5.0709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3070,13 +3070,13 @@
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>1.8556</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>1.8556</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
@@ -3122,43 +3122,43 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.0263</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
         <v>0.0075</v>
       </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0.0263</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="n">
-        <v>0</v>
-      </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>0.0038</v>
       </c>
       <c r="T37" t="n">
         <v>0</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="W37" t="n">
-        <v>0.0038</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3225,25 +3225,25 @@
         <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>0.168</v>
       </c>
       <c r="R38" t="n">
         <v>0</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="T38" t="n">
         <v>0</v>
       </c>
       <c r="U38" t="n">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="V38" t="n">
         <v>0</v>
       </c>
       <c r="W38" t="n">
-        <v>0.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3283,13 +3283,13 @@
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>0.0985</v>
       </c>
       <c r="M39" t="n">
         <v>0.1675</v>
       </c>
       <c r="N39" t="n">
-        <v>0.0985</v>
+        <v>0</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -3298,25 +3298,25 @@
         <v>0</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="R39" t="n">
         <v>0</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>0.0197</v>
       </c>
       <c r="T39" t="n">
         <v>0</v>
       </c>
       <c r="U39" t="n">
-        <v>0.009900000000000001</v>
+        <v>0</v>
       </c>
       <c r="V39" t="n">
         <v>0</v>
       </c>
       <c r="W39" t="n">
-        <v>0.0197</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3414,43 +3414,43 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
         <v>0.0013</v>
       </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="n">
-        <v>0</v>
-      </c>
       <c r="S41" t="n">
-        <v>0</v>
+        <v>6.0048</v>
       </c>
       <c r="T41" t="n">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="W41" t="n">
-        <v>6.0048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3502,13 +3502,13 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>0.0431</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0.0431</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5569</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -3575,22 +3575,22 @@
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0497</v>
+        <v>0</v>
       </c>
       <c r="M43" t="n">
         <v>1.2529</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>0.0139</v>
       </c>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>0.5569</v>
       </c>
       <c r="P43" t="n">
-        <v>0.0139</v>
+        <v>0</v>
       </c>
       <c r="Q43" t="n">
-        <v>0</v>
+        <v>0.0975</v>
       </c>
       <c r="R43" t="n">
         <v>0</v>
@@ -3602,13 +3602,13 @@
         <v>0</v>
       </c>
       <c r="U43" t="n">
-        <v>0.0975</v>
+        <v>0</v>
       </c>
       <c r="V43" t="n">
         <v>0</v>
       </c>
       <c r="W43" t="n">
-        <v>0</v>
+        <v>0.0497</v>
       </c>
     </row>
     <row r="44">
@@ -3648,13 +3648,13 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>0.0281</v>
       </c>
       <c r="M44" t="n">
         <v>0.014</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0281</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
         <v>0</v>
@@ -3663,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="R44" t="n">
         <v>0</v>
@@ -3675,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="U44" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="V44" t="n">
         <v>0</v>
@@ -3727,13 +3727,13 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>1.66</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="n">
         <v>0</v>
@@ -3770,64 +3770,64 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
+        <v>0.0074</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.0731</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.9147999999999999</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.4638</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.335</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.8375</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
         <v>3.7401</v>
       </c>
-      <c r="E46" t="n">
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0.5062</v>
+      </c>
+      <c r="T46" t="n">
         <v>9.5472</v>
       </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.2043</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="n">
-        <v>1.0731</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" t="n">
-        <v>0.8375</v>
-      </c>
-      <c r="O46" t="n">
-        <v>0.0074</v>
-      </c>
-      <c r="P46" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q46" t="n">
+      <c r="U46" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="V46" t="n">
         <v>0.0018</v>
       </c>
-      <c r="R46" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="S46" t="n">
-        <v>0.4638</v>
-      </c>
-      <c r="T46" t="n">
-        <v>0.0037</v>
-      </c>
-      <c r="U46" t="n">
-        <v>0</v>
-      </c>
-      <c r="V46" t="n">
-        <v>0.9147999999999999</v>
-      </c>
       <c r="W46" t="n">
-        <v>0.5062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3940,13 +3940,13 @@
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>0.0109</v>
       </c>
       <c r="M48" t="n">
         <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0109</v>
+        <v>0</v>
       </c>
       <c r="O48" t="n">
         <v>0</v>
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="S48" t="n">
-        <v>0</v>
+        <v>0.2437</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
       <c r="W48" t="n">
-        <v>0.2437</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -3998,40 +3998,40 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" t="n">
         <v>0.0008</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" t="n">
-        <v>0</v>
-      </c>
-      <c r="O49" t="n">
-        <v>0</v>
-      </c>
-      <c r="P49" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q49" t="n">
-        <v>0</v>
-      </c>
-      <c r="R49" t="n">
-        <v>0</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0019</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -4159,13 +4159,13 @@
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>2.6374</v>
       </c>
       <c r="M51" t="n">
         <v>0.0057</v>
       </c>
       <c r="N51" t="n">
-        <v>2.6374</v>
+        <v>0</v>
       </c>
       <c r="O51" t="n">
         <v>0</v>
@@ -4177,10 +4177,10 @@
         <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.0019</v>
       </c>
       <c r="S51" t="n">
-        <v>0</v>
+        <v>0.0019</v>
       </c>
       <c r="T51" t="n">
         <v>0</v>
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -4311,13 +4311,13 @@
         <v>0.0185</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>0.3405</v>
       </c>
       <c r="O53" t="n">
         <v>0</v>
       </c>
       <c r="P53" t="n">
-        <v>0.3405</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="n">
         <v>0</v>
@@ -4354,64 +4354,64 @@
         <v>1</v>
       </c>
       <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.0463</v>
+      </c>
+      <c r="H54" t="n">
         <v>0.0154</v>
       </c>
-      <c r="E54" t="n">
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1.2645</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0.3547</v>
+      </c>
+      <c r="T54" t="n">
         <v>0.0308</v>
       </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0</v>
-      </c>
-      <c r="K54" t="n">
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" t="n">
         <v>0.0154</v>
       </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
-        <v>0</v>
-      </c>
-      <c r="P54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q54" t="n">
-        <v>0.0154</v>
-      </c>
-      <c r="R54" t="n">
-        <v>1.2645</v>
-      </c>
-      <c r="S54" t="n">
-        <v>0.0463</v>
-      </c>
-      <c r="T54" t="n">
-        <v>0</v>
-      </c>
-      <c r="U54" t="n">
-        <v>0</v>
-      </c>
-      <c r="V54" t="n">
-        <v>0</v>
-      </c>
       <c r="W54" t="n">
-        <v>0.3547</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4427,64 +4427,64 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>0.1537</v>
       </c>
       <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.1153</v>
+      </c>
+      <c r="H55" t="n">
+        <v>8.9337</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1.3641</v>
+      </c>
+      <c r="K55" t="n">
+        <v>3.1508</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.1921</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>1.3256</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0.07679999999999999</v>
+      </c>
+      <c r="T55" t="n">
         <v>0.1537</v>
       </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1.3256</v>
-      </c>
-      <c r="H55" t="n">
-        <v>3.1508</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>8.9337</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" t="n">
-        <v>0.1921</v>
-      </c>
-      <c r="O55" t="n">
-        <v>0.1537</v>
-      </c>
-      <c r="P55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q55" t="n">
+      <c r="U55" t="n">
+        <v>0.0384</v>
+      </c>
+      <c r="V55" t="n">
         <v>2.7089</v>
       </c>
-      <c r="R55" t="n">
-        <v>1.3641</v>
-      </c>
-      <c r="S55" t="n">
-        <v>0.1153</v>
-      </c>
-      <c r="T55" t="n">
-        <v>0.0384</v>
-      </c>
-      <c r="U55" t="n">
-        <v>0</v>
-      </c>
-      <c r="V55" t="n">
-        <v>0</v>
-      </c>
       <c r="W55" t="n">
-        <v>0.07679999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -4500,64 +4500,64 @@
         <v>1</v>
       </c>
       <c r="D56" t="n">
+        <v>0.1331</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.0526</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.0385</v>
+      </c>
+      <c r="H56" t="n">
+        <v>10.5735</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1.2613</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3.6191</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.1717</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
         <v>0.007</v>
       </c>
-      <c r="E56" t="n">
+      <c r="Q56" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0.9459</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="T56" t="n">
         <v>0.0911</v>
       </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0.9459</v>
-      </c>
-      <c r="H56" t="n">
-        <v>3.6191</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0.0526</v>
-      </c>
-      <c r="K56" t="n">
-        <v>10.5735</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
-        <v>0.1717</v>
-      </c>
-      <c r="O56" t="n">
-        <v>0.1331</v>
-      </c>
-      <c r="P56" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q56" t="n">
+      <c r="U56" t="n">
+        <v>0.1086</v>
+      </c>
+      <c r="V56" t="n">
         <v>3.0515</v>
       </c>
-      <c r="R56" t="n">
-        <v>1.2613</v>
-      </c>
-      <c r="S56" t="n">
-        <v>0.0385</v>
-      </c>
-      <c r="T56" t="n">
-        <v>0.1086</v>
-      </c>
-      <c r="U56" t="n">
-        <v>0</v>
-      </c>
-      <c r="V56" t="n">
-        <v>0.035</v>
-      </c>
       <c r="W56" t="n">
-        <v>0.049</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4597,13 +4597,13 @@
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>0.98</v>
+        <v>0</v>
       </c>
       <c r="O57" t="n">
         <v>0</v>
@@ -4646,64 +4646,64 @@
         <v>1</v>
       </c>
       <c r="D58" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.1174</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.0587</v>
+      </c>
+      <c r="K58" t="n">
         <v>0.0053</v>
       </c>
-      <c r="E58" t="n">
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>4.7884</v>
+      </c>
+      <c r="T58" t="n">
         <v>0.0391</v>
       </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.0053</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" t="n">
-        <v>0</v>
-      </c>
-      <c r="K58" t="n">
-        <v>0</v>
-      </c>
-      <c r="L58" t="n">
-        <v>0</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" t="n">
-        <v>0</v>
-      </c>
-      <c r="O58" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="P58" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q58" t="n">
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
+      <c r="V58" t="n">
         <v>0.0338</v>
       </c>
-      <c r="R58" t="n">
-        <v>0.0587</v>
-      </c>
-      <c r="S58" t="n">
-        <v>0.1174</v>
-      </c>
-      <c r="T58" t="n">
-        <v>0</v>
-      </c>
-      <c r="U58" t="n">
-        <v>0</v>
-      </c>
-      <c r="V58" t="n">
-        <v>0.0036</v>
-      </c>
       <c r="W58" t="n">
-        <v>4.7884</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -4728,41 +4728,41 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.1488</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="R59" t="n">
         <v>0.2975</v>
       </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0</v>
-      </c>
-      <c r="K59" t="n">
-        <v>0</v>
-      </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" t="n">
-        <v>0.1488</v>
-      </c>
-      <c r="O59" t="n">
-        <v>0</v>
-      </c>
-      <c r="P59" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q59" t="n">
-        <v>0</v>
-      </c>
-      <c r="R59" t="n">
-        <v>0</v>
-      </c>
       <c r="S59" t="n">
         <v>0</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="U59" t="n">
-        <v>0.502</v>
+        <v>0</v>
       </c>
       <c r="V59" t="n">
         <v>0</v>
@@ -4801,7 +4801,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>1.1426</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -4816,13 +4816,13 @@
         <v>0</v>
       </c>
       <c r="L60" t="n">
-        <v>0</v>
+        <v>0.9507</v>
       </c>
       <c r="M60" t="n">
         <v>0.0044</v>
       </c>
       <c r="N60" t="n">
-        <v>0.9507</v>
+        <v>0</v>
       </c>
       <c r="O60" t="n">
         <v>0</v>
@@ -4831,25 +4831,25 @@
         <v>0</v>
       </c>
       <c r="Q60" t="n">
-        <v>0</v>
+        <v>0.0218</v>
       </c>
       <c r="R60" t="n">
-        <v>0</v>
+        <v>1.1426</v>
       </c>
       <c r="S60" t="n">
-        <v>0</v>
+        <v>0.0131</v>
       </c>
       <c r="T60" t="n">
         <v>0</v>
       </c>
       <c r="U60" t="n">
-        <v>0.0218</v>
+        <v>0</v>
       </c>
       <c r="V60" t="n">
         <v>0</v>
       </c>
       <c r="W60" t="n">
-        <v>0.0131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -4874,40 +4874,40 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.6935</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" t="n">
         <v>1.1096</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" t="n">
-        <v>0.6935</v>
-      </c>
-      <c r="O61" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q61" t="n">
-        <v>0</v>
-      </c>
-      <c r="R61" t="n">
-        <v>0</v>
       </c>
       <c r="S61" t="n">
         <v>0</v>
@@ -4947,40 +4947,40 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0</v>
+      </c>
+      <c r="R62" t="n">
         <v>7.76</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="O62" t="n">
-        <v>0</v>
-      </c>
-      <c r="P62" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q62" t="n">
-        <v>0</v>
-      </c>
-      <c r="R62" t="n">
-        <v>0</v>
       </c>
       <c r="S62" t="n">
         <v>0</v>
@@ -5056,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="S63" t="n">
-        <v>0</v>
+        <v>0.4355</v>
       </c>
       <c r="T63" t="n">
         <v>0</v>
@@ -5068,7 +5068,7 @@
         <v>0</v>
       </c>
       <c r="W63" t="n">
-        <v>0.4355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -5093,40 +5093,40 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" t="n">
         <v>2.18</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K64" t="n">
-        <v>0</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" t="n">
-        <v>0</v>
-      </c>
-      <c r="N64" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="O64" t="n">
-        <v>0</v>
-      </c>
-      <c r="P64" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q64" t="n">
-        <v>0</v>
-      </c>
-      <c r="R64" t="n">
-        <v>0</v>
       </c>
       <c r="S64" t="n">
         <v>0</v>
@@ -5269,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>0</v>
+        <v>0.0688</v>
       </c>
       <c r="R66" t="n">
         <v>0</v>
@@ -5281,7 +5281,7 @@
         <v>0</v>
       </c>
       <c r="U66" t="n">
-        <v>0.0688</v>
+        <v>0</v>
       </c>
       <c r="V66" t="n">
         <v>0</v>
@@ -5312,40 +5312,40 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>5.11</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" t="n">
         <v>5.23</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I67" t="n">
-        <v>0</v>
-      </c>
-      <c r="J67" t="n">
-        <v>0</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="n">
-        <v>0</v>
-      </c>
-      <c r="N67" t="n">
-        <v>0</v>
-      </c>
-      <c r="O67" t="n">
-        <v>0</v>
-      </c>
-      <c r="P67" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q67" t="n">
-        <v>0</v>
-      </c>
-      <c r="R67" t="n">
-        <v>5.11</v>
       </c>
       <c r="S67" t="n">
         <v>0</v>
@@ -5385,43 +5385,43 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>3.0508</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" t="n">
         <v>0.2183</v>
       </c>
-      <c r="H68" t="n">
-        <v>0</v>
-      </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="n">
-        <v>0</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" t="n">
-        <v>0</v>
-      </c>
-      <c r="N68" t="n">
-        <v>3.0508</v>
-      </c>
-      <c r="O68" t="n">
-        <v>0</v>
-      </c>
-      <c r="P68" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q68" t="n">
-        <v>0</v>
-      </c>
-      <c r="R68" t="n">
-        <v>0</v>
-      </c>
       <c r="S68" t="n">
-        <v>0</v>
+        <v>0.3686</v>
       </c>
       <c r="T68" t="n">
         <v>0</v>
@@ -5433,7 +5433,7 @@
         <v>0</v>
       </c>
       <c r="W68" t="n">
-        <v>0.3686</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -5467,7 +5467,7 @@
         <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="K69" t="n">
         <v>0</v>
@@ -5491,16 +5491,16 @@
         <v>0</v>
       </c>
       <c r="R69" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="S69" t="n">
         <v>0</v>
       </c>
       <c r="T69" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="n">
         <v>2.3</v>
-      </c>
-      <c r="U69" t="n">
-        <v>0</v>
       </c>
       <c r="V69" t="n">
         <v>0</v>
@@ -5561,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="Q70" t="n">
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="R70" t="n">
         <v>0</v>
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="U70" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="V70" t="n">
         <v>0</v>
@@ -5625,16 +5625,16 @@
         <v>0</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>0.1935</v>
       </c>
       <c r="O71" t="n">
         <v>0</v>
       </c>
       <c r="P71" t="n">
-        <v>0.1935</v>
+        <v>0</v>
       </c>
       <c r="Q71" t="n">
-        <v>0</v>
+        <v>0.0506</v>
       </c>
       <c r="R71" t="n">
         <v>0</v>
@@ -5646,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="U71" t="n">
-        <v>0.0506</v>
+        <v>0</v>
       </c>
       <c r="V71" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
new dfs pca, regression, classification
</commit_message>
<xml_diff>
--- a/data/Influencers_OLS.xlsx
+++ b/data/Influencers_OLS.xlsx
@@ -446,102 +446,102 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>863</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>408</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>526</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>725</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>214</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>871</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>678</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>712</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>471</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>229</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>625</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>864</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>712</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>214</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>549</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>625</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>863</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>229</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>526</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>584</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>725</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>408</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>351</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>375</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>334</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>871</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>471</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.1508</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1508</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -637,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -670,13 +670,13 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>2.42</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -710,20 +710,20 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.2047</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0767</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.0767</v>
       </c>
       <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.921</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
@@ -731,19 +731,19 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>5.8839</v>
+      </c>
+      <c r="P4" t="n">
         <v>11.9724</v>
       </c>
-      <c r="N4" t="n">
-        <v>0.0767</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.0767</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
       <c r="Q4" t="n">
-        <v>0.2047</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>5.8839</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -783,20 +783,20 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.07489999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.0336</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.1188</v>
       </c>
       <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.3021</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
@@ -804,19 +804,19 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.1592</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.1394</v>
       </c>
-      <c r="N5" t="n">
-        <v>0.0336</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.1188</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
       <c r="Q5" t="n">
-        <v>0.07489999999999999</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>1.1592</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -856,20 +856,20 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>3.156</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.0595</v>
       </c>
       <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
         <v>0.6947</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
@@ -877,19 +877,19 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5558</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.8535</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.0595</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
       <c r="Q6" t="n">
-        <v>3.156</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>0.5558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -929,20 +929,20 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.168</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.2431</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
         <v>13.5058</v>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1512</v>
+      </c>
+      <c r="P7" t="n">
         <v>4.9051</v>
       </c>
-      <c r="N7" t="n">
-        <v>1.2431</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.0504</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
       <c r="Q7" t="n">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0.1512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1002,20 +1002,20 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.3127</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1.2749</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2.3622</v>
       </c>
       <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
         <v>3.6515</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
@@ -1023,19 +1023,19 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.3656</v>
+      </c>
+      <c r="P8" t="n">
         <v>2.7326</v>
       </c>
-      <c r="N8" t="n">
-        <v>1.2749</v>
-      </c>
-      <c r="O8" t="n">
-        <v>2.3622</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
       <c r="Q8" t="n">
-        <v>0.3127</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.3656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1075,20 +1075,20 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>3.4666</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.1686</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.08550000000000001</v>
       </c>
       <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
         <v>0.9429999999999999</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -1096,19 +1096,19 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.2541</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.9258999999999999</v>
       </c>
-      <c r="N9" t="n">
-        <v>0.1686</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.08550000000000001</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
       <c r="Q9" t="n">
-        <v>3.4666</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>0.2541</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1151,28 +1151,28 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
         <v>0.1059</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
@@ -1215,64 +1215,64 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0126</v>
+        <v>1.661</v>
       </c>
       <c r="E11" t="n">
         <v>0.2643</v>
       </c>
       <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1762</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.2517</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.151</v>
       </c>
-      <c r="G11" t="n">
-        <v>0.2517</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
+      <c r="S11" t="n">
+        <v>1.8498</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="U11" t="n">
         <v>2.7054</v>
       </c>
-      <c r="K11" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.661</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.1762</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>1.8498</v>
-      </c>
-      <c r="S11" t="n">
+      <c r="V11" t="n">
         <v>0.4404</v>
       </c>
-      <c r="T11" t="n">
+      <c r="W11" t="n">
         <v>0.7927999999999999</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1315,16 +1315,16 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.0029</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
@@ -1361,64 +1361,64 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>2.1628</v>
       </c>
       <c r="E13" t="n">
         <v>0.2466</v>
       </c>
       <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.3035</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3.2821</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
         <v>1.2332</v>
       </c>
-      <c r="G13" t="n">
-        <v>3.2821</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
+      <c r="S13" t="n">
+        <v>0.1138</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
         <v>0.3035</v>
       </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>2.1628</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.3035</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.1138</v>
-      </c>
-      <c r="S13" t="n">
+      <c r="V13" t="n">
         <v>0.6261</v>
       </c>
-      <c r="T13" t="n">
+      <c r="W13" t="n">
         <v>0.702</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1476,10 +1476,10 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>0.0144</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1528,25 +1528,25 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
         <v>0.295</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.0047</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
       </c>
       <c r="R15" t="n">
         <v>0</v>
@@ -1586,20 +1586,20 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.4334</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.0867</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>0.1326</v>
       </c>
       <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
         <v>1.3715</v>
       </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
@@ -1607,19 +1607,19 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.7877</v>
+      </c>
+      <c r="P16" t="n">
         <v>0.8999</v>
       </c>
-      <c r="N16" t="n">
-        <v>0.0867</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.1326</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
       <c r="Q16" t="n">
-        <v>0.4334</v>
+        <v>0</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>0.7877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.3597</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1668,11 +1668,11 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
         <v>3.2514</v>
       </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
@@ -1680,19 +1680,19 @@
         <v>0</v>
       </c>
       <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
         <v>2.605</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0</v>
-      </c>
       <c r="Q17" t="n">
-        <v>0.3597</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -1726,58 +1726,58 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.0298</v>
       </c>
       <c r="E18" t="n">
         <v>0.005</v>
       </c>
       <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
         <v>0.005</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
+      <c r="R18" t="n">
         <v>0.005</v>
       </c>
-      <c r="L18" t="n">
-        <v>0.0298</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>0.0944</v>
       </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="U18" t="n">
-        <v>0.009900000000000001</v>
+        <v>0</v>
       </c>
       <c r="V18" t="n">
         <v>0</v>
@@ -1799,13 +1799,13 @@
         <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.3076</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.0259</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1823,37 +1823,37 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0.3076</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
         <v>0.0029</v>
       </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
       <c r="Q19" t="n">
-        <v>0.0259</v>
+        <v>0</v>
       </c>
       <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
         <v>0.8107</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="n">
         <v>0.06610000000000001</v>
-      </c>
-      <c r="T19" t="n">
-        <v>0</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" t="n">
-        <v>0</v>
       </c>
       <c r="W19" t="n">
         <v>0</v>
@@ -1890,40 +1890,40 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
         <v>0.3998</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.0013</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" t="n">
-        <v>0</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0</v>
       </c>
       <c r="V20" t="n">
         <v>0</v>
@@ -1990,16 +1990,16 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
         <v>0.0016</v>
-      </c>
-      <c r="T21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
       </c>
       <c r="W21" t="n">
         <v>0</v>
@@ -2018,64 +2018,64 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>1.4986</v>
+        <v>0.2191</v>
       </c>
       <c r="E22" t="n">
         <v>0.0117</v>
       </c>
       <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0078</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.4069</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1.4986</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1.4751</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.4617</v>
+      </c>
+      <c r="R22" t="n">
         <v>0.0391</v>
       </c>
-      <c r="G22" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1.4751</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
+      <c r="S22" t="n">
+        <v>5.1571</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1.7373</v>
+      </c>
+      <c r="U22" t="n">
         <v>7.1605</v>
       </c>
-      <c r="K22" t="n">
-        <v>0.4617</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.2191</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0.0078</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>5.1571</v>
-      </c>
-      <c r="S22" t="n">
+      <c r="V22" t="n">
         <v>0.0157</v>
       </c>
-      <c r="T22" t="n">
+      <c r="W22" t="n">
         <v>0.1683</v>
-      </c>
-      <c r="U22" t="n">
-        <v>1.7373</v>
-      </c>
-      <c r="V22" t="n">
-        <v>0.4069</v>
-      </c>
-      <c r="W22" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2097,20 +2097,20 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.2687</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.0192</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>1.8231</v>
       </c>
       <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
         <v>0.1151</v>
       </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
       <c r="K23" t="n">
         <v>0</v>
       </c>
@@ -2118,19 +2118,19 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.1343</v>
+      </c>
+      <c r="P23" t="n">
         <v>0.5757</v>
       </c>
-      <c r="N23" t="n">
-        <v>0.0192</v>
-      </c>
-      <c r="O23" t="n">
-        <v>1.8231</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
-      </c>
       <c r="Q23" t="n">
-        <v>0.2687</v>
+        <v>0</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -2148,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>0.1343</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2164,64 +2164,64 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.8102</v>
       </c>
       <c r="E24" t="n">
         <v>1.4854</v>
       </c>
       <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3.5846</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.2946</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
         <v>0.3069</v>
       </c>
-      <c r="G24" t="n">
-        <v>0.2946</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.0123</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
+      <c r="S24" t="n">
+        <v>0.2332</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
         <v>0.3069</v>
       </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.8102</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>3.5846</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0.2332</v>
-      </c>
-      <c r="S24" t="n">
+      <c r="V24" t="n">
         <v>0.4297</v>
       </c>
-      <c r="T24" t="n">
+      <c r="W24" t="n">
         <v>0.6875</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.1704</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -2252,11 +2252,11 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
         <v>0.1928</v>
       </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
       <c r="K25" t="n">
         <v>0</v>
       </c>
@@ -2264,34 +2264,34 @@
         <v>0</v>
       </c>
       <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
         <v>0.1748</v>
       </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
       <c r="Q25" t="n">
-        <v>0.1704</v>
+        <v>0</v>
       </c>
       <c r="R25" t="n">
         <v>0</v>
       </c>
       <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
         <v>0.7262999999999999</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
       </c>
       <c r="W25" t="n">
         <v>0</v>
@@ -2389,10 +2389,10 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>0.0395</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.0395</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2410,19 +2410,19 @@
         <v>0</v>
       </c>
       <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
         <v>0.06909999999999999</v>
       </c>
-      <c r="N27" t="n">
-        <v>0.0395</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
-      </c>
       <c r="Q27" t="n">
-        <v>0.0395</v>
+        <v>0</v>
       </c>
       <c r="R27" t="n">
         <v>0</v>
@@ -2456,13 +2456,13 @@
         <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>0.948</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>0.0271</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>0.948</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
         <v>0</v>
@@ -2495,13 +2495,13 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.0271</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
         <v>0.5959</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
       </c>
       <c r="T28" t="n">
         <v>0</v>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -2556,16 +2556,16 @@
         <v>0</v>
       </c>
       <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
         <v>0.55</v>
-      </c>
-      <c r="N29" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
@@ -2602,7 +2602,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>3.0972</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
         <v>0.2099</v>
@@ -2620,46 +2620,46 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>3.0972</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
         <v>1.4328</v>
       </c>
-      <c r="K30" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="n">
-        <v>0.0145</v>
-      </c>
-      <c r="S30" t="n">
+      <c r="V30" t="n">
         <v>0.0579</v>
       </c>
-      <c r="T30" t="n">
+      <c r="W30" t="n">
         <v>0.5934</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0</v>
-      </c>
-      <c r="W30" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2675,13 +2675,13 @@
         <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>0.4151</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>0.0511</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0.4151</v>
+        <v>0</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
@@ -2714,22 +2714,22 @@
         <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.0511</v>
+        <v>0</v>
       </c>
       <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
         <v>0.2917</v>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
         <v>0.003</v>
-      </c>
-      <c r="T31" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0</v>
       </c>
       <c r="W31" t="n">
         <v>0</v>
@@ -2748,13 +2748,13 @@
         <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>0.8921</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>0.0277</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>0.8921</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
         <v>0</v>
@@ -2787,22 +2787,22 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.0277</v>
+        <v>0</v>
       </c>
       <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
         <v>0.1908</v>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
         <v>0.008200000000000001</v>
-      </c>
-      <c r="T32" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>0</v>
       </c>
       <c r="W32" t="n">
         <v>0</v>
@@ -2821,13 +2821,13 @@
         <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>0.0107</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>0.0129</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -2836,46 +2836,46 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
         <v>0.5633</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
       <c r="K33" t="n">
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0107</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
         <v>0.0493</v>
       </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
       <c r="Q33" t="n">
-        <v>0.0129</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>0</v>
       </c>
       <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
         <v>0.0278</v>
-      </c>
-      <c r="T33" t="n">
-        <v>0</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0</v>
       </c>
       <c r="W33" t="n">
         <v>0</v>
@@ -2894,13 +2894,13 @@
         <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>0.0182</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>0.1065</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -2909,46 +2909,46 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
         <v>0.0774</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
       <c r="K34" t="n">
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0182</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
         <v>0.19</v>
       </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" t="n">
-        <v>0</v>
-      </c>
       <c r="Q34" t="n">
-        <v>0.1065</v>
+        <v>0</v>
       </c>
       <c r="R34" t="n">
         <v>0</v>
       </c>
       <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
         <v>0.0339</v>
-      </c>
-      <c r="T34" t="n">
-        <v>0</v>
-      </c>
-      <c r="U34" t="n">
-        <v>0</v>
-      </c>
-      <c r="V34" t="n">
-        <v>0</v>
       </c>
       <c r="W34" t="n">
         <v>0</v>
@@ -2967,64 +2967,64 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>1.536</v>
       </c>
       <c r="E35" t="n">
         <v>4.4009</v>
       </c>
       <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2.0539</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2.8605</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.0044</v>
+      </c>
+      <c r="R35" t="n">
         <v>2.2016</v>
       </c>
-      <c r="G35" t="n">
-        <v>2.8605</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
+      <c r="S35" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.0022</v>
+      </c>
+      <c r="U35" t="n">
         <v>0.2292</v>
       </c>
-      <c r="K35" t="n">
-        <v>0.0044</v>
-      </c>
-      <c r="L35" t="n">
-        <v>1.536</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" t="n">
-        <v>2.0539</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="S35" t="n">
+      <c r="V35" t="n">
         <v>5.0709</v>
       </c>
-      <c r="T35" t="n">
+      <c r="W35" t="n">
         <v>0.6016</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0.0022</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1.8556</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3070,7 +3070,7 @@
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>1.8556</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>0.0263</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -3137,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0263</v>
+        <v>0</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
@@ -3155,19 +3155,19 @@
         <v>0</v>
       </c>
       <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
         <v>0.0075</v>
       </c>
-      <c r="S37" t="n">
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
         <v>0.0038</v>
-      </c>
-      <c r="T37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>0</v>
       </c>
       <c r="W37" t="n">
         <v>0</v>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>0.168</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -3201,11 +3201,11 @@
         <v>0</v>
       </c>
       <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
         <v>4.2629</v>
       </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
       <c r="K38" t="n">
         <v>0</v>
       </c>
@@ -3213,34 +3213,34 @@
         <v>0</v>
       </c>
       <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
         <v>1.008</v>
       </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
       <c r="Q38" t="n">
-        <v>0.168</v>
+        <v>0</v>
       </c>
       <c r="R38" t="n">
         <v>0</v>
       </c>
       <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
         <v>0.63</v>
-      </c>
-      <c r="T38" t="n">
-        <v>0</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>0</v>
       </c>
       <c r="W38" t="n">
         <v>0</v>
@@ -3259,13 +3259,13 @@
         <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>0.0985</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -3274,46 +3274,46 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
         <v>0.0493</v>
       </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
       <c r="K39" t="n">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>0.0985</v>
+        <v>0</v>
       </c>
       <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
         <v>0.1675</v>
       </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
       <c r="Q39" t="n">
-        <v>0.009900000000000001</v>
+        <v>0</v>
       </c>
       <c r="R39" t="n">
         <v>0</v>
       </c>
       <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
         <v>0.0197</v>
-      </c>
-      <c r="T39" t="n">
-        <v>0</v>
-      </c>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>0</v>
       </c>
       <c r="W39" t="n">
         <v>0</v>
@@ -3347,10 +3347,10 @@
         <v>0</v>
       </c>
       <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
         <v>4.41</v>
-      </c>
-      <c r="J40" t="n">
-        <v>0</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -3447,19 +3447,19 @@
         <v>0</v>
       </c>
       <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
         <v>0.0013</v>
       </c>
-      <c r="S41" t="n">
+      <c r="T41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="n">
         <v>6.0048</v>
-      </c>
-      <c r="T41" t="n">
-        <v>0</v>
-      </c>
-      <c r="U41" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" t="n">
-        <v>0</v>
       </c>
       <c r="W41" t="n">
         <v>0</v>
@@ -3478,7 +3478,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>0.0431</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -3502,7 +3502,7 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0431</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -3557,20 +3557,20 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>0.0975</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>0.0139</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>0.5569</v>
       </c>
       <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
         <v>0.0975</v>
       </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
       <c r="K43" t="n">
         <v>0</v>
       </c>
@@ -3578,19 +3578,19 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.0497</v>
+      </c>
+      <c r="P43" t="n">
         <v>1.2529</v>
       </c>
-      <c r="N43" t="n">
-        <v>0.0139</v>
-      </c>
-      <c r="O43" t="n">
-        <v>0.5569</v>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
       <c r="Q43" t="n">
-        <v>0.0975</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
         <v>0</v>
@@ -3608,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="W43" t="n">
-        <v>0.0497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -3624,13 +3624,13 @@
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.0281</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -3639,31 +3639,31 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
         <v>0.1264</v>
       </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
       <c r="K44" t="n">
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0281</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
         <v>0.014</v>
       </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
-        <v>0</v>
-      </c>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
       <c r="Q44" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="R44" t="n">
         <v>0</v>
@@ -3706,17 +3706,17 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
       </c>
       <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
         <v>5.7</v>
       </c>
-      <c r="J45" t="n">
-        <v>0</v>
-      </c>
       <c r="K45" t="n">
         <v>0</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>1.66</v>
+        <v>0</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -3770,64 +3770,64 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0074</v>
+        <v>0.8375</v>
       </c>
       <c r="E46" t="n">
         <v>1.0731</v>
       </c>
       <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3.7401</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.0074</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.4638</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
         <v>0.9147999999999999</v>
       </c>
-      <c r="G46" t="n">
-        <v>0.4638</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="n">
+      <c r="S46" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="U46" t="n">
         <v>0.335</v>
       </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0.8375</v>
-      </c>
-      <c r="M46" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" t="n">
-        <v>0</v>
-      </c>
-      <c r="O46" t="n">
-        <v>0</v>
-      </c>
-      <c r="P46" t="n">
-        <v>3.7401</v>
-      </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" t="n">
-        <v>0.2043</v>
-      </c>
-      <c r="S46" t="n">
+      <c r="V46" t="n">
         <v>0.5062</v>
       </c>
-      <c r="T46" t="n">
+      <c r="W46" t="n">
         <v>9.5472</v>
-      </c>
-      <c r="U46" t="n">
-        <v>0.0037</v>
-      </c>
-      <c r="V46" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="W46" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3916,7 +3916,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>0.0109</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0109</v>
+        <v>0</v>
       </c>
       <c r="M48" t="n">
         <v>0</v>
@@ -3961,16 +3961,16 @@
         <v>0</v>
       </c>
       <c r="S48" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" t="n">
         <v>0.2437</v>
-      </c>
-      <c r="T48" t="n">
-        <v>0</v>
-      </c>
-      <c r="U48" t="n">
-        <v>0</v>
-      </c>
-      <c r="V48" t="n">
-        <v>0</v>
       </c>
       <c r="W48" t="n">
         <v>0</v>
@@ -4031,10 +4031,10 @@
         <v>0</v>
       </c>
       <c r="R49" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="n">
         <v>0.0008</v>
-      </c>
-      <c r="S49" t="n">
-        <v>0</v>
       </c>
       <c r="T49" t="n">
         <v>0</v>
@@ -4135,7 +4135,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>2.6374</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -4159,25 +4159,25 @@
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>2.6374</v>
+        <v>0</v>
       </c>
       <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
         <v>0.0057</v>
       </c>
-      <c r="N51" t="n">
-        <v>0</v>
-      </c>
-      <c r="O51" t="n">
-        <v>0</v>
-      </c>
-      <c r="P51" t="n">
-        <v>0</v>
-      </c>
       <c r="Q51" t="n">
         <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>0.0019</v>
+        <v>0</v>
       </c>
       <c r="S51" t="n">
         <v>0.0019</v>
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="V51" t="n">
-        <v>0</v>
+        <v>0.0019</v>
       </c>
       <c r="W51" t="n">
         <v>0</v>
@@ -4235,16 +4235,16 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
         <v>0.0035</v>
-      </c>
-      <c r="N52" t="n">
-        <v>0</v>
-      </c>
-      <c r="O52" t="n">
-        <v>0</v>
-      </c>
-      <c r="P52" t="n">
-        <v>0</v>
       </c>
       <c r="Q52" t="n">
         <v>0</v>
@@ -4290,7 +4290,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>0.3405</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4308,16 +4308,16 @@
         <v>0</v>
       </c>
       <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
         <v>0.0185</v>
-      </c>
-      <c r="N53" t="n">
-        <v>0.3405</v>
-      </c>
-      <c r="O53" t="n">
-        <v>0</v>
-      </c>
-      <c r="P53" t="n">
-        <v>0</v>
       </c>
       <c r="Q53" t="n">
         <v>0</v>
@@ -4363,55 +4363,55 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="N54" t="n">
         <v>0.0463</v>
       </c>
-      <c r="H54" t="n">
-        <v>0.0154</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="n">
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0</v>
+      </c>
+      <c r="T54" t="n">
+        <v>0</v>
+      </c>
+      <c r="U54" t="n">
         <v>1.2645</v>
       </c>
-      <c r="K54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
-        <v>0</v>
-      </c>
-      <c r="P54" t="n">
-        <v>0.0154</v>
-      </c>
-      <c r="Q54" t="n">
-        <v>0</v>
-      </c>
-      <c r="R54" t="n">
-        <v>0</v>
-      </c>
-      <c r="S54" t="n">
+      <c r="V54" t="n">
         <v>0.3547</v>
       </c>
-      <c r="T54" t="n">
+      <c r="W54" t="n">
         <v>0.0308</v>
-      </c>
-      <c r="U54" t="n">
-        <v>0</v>
-      </c>
-      <c r="V54" t="n">
-        <v>0.0154</v>
-      </c>
-      <c r="W54" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4427,64 +4427,64 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
+        <v>0.1921</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2.7089</v>
+      </c>
+      <c r="L55" t="n">
         <v>0.1537</v>
       </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
+      <c r="M55" t="n">
+        <v>8.9337</v>
+      </c>
+      <c r="N55" t="n">
         <v>0.1153</v>
       </c>
-      <c r="H55" t="n">
-        <v>8.9337</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>3.1508</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>1.3256</v>
+      </c>
+      <c r="T55" t="n">
+        <v>0.0384</v>
+      </c>
+      <c r="U55" t="n">
         <v>1.3641</v>
       </c>
-      <c r="K55" t="n">
-        <v>3.1508</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0.1921</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" t="n">
-        <v>0</v>
-      </c>
-      <c r="O55" t="n">
-        <v>0</v>
-      </c>
-      <c r="P55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q55" t="n">
-        <v>0</v>
-      </c>
-      <c r="R55" t="n">
-        <v>1.3256</v>
-      </c>
-      <c r="S55" t="n">
+      <c r="V55" t="n">
         <v>0.07679999999999999</v>
       </c>
-      <c r="T55" t="n">
+      <c r="W55" t="n">
         <v>0.1537</v>
-      </c>
-      <c r="U55" t="n">
-        <v>0.0384</v>
-      </c>
-      <c r="V55" t="n">
-        <v>2.7089</v>
-      </c>
-      <c r="W55" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -4500,64 +4500,64 @@
         <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1331</v>
+        <v>0.1717</v>
       </c>
       <c r="E56" t="n">
         <v>0.0526</v>
       </c>
       <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3.0515</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.1331</v>
+      </c>
+      <c r="M56" t="n">
+        <v>10.5735</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.0385</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>3.6191</v>
+      </c>
+      <c r="R56" t="n">
         <v>0.035</v>
       </c>
-      <c r="G56" t="n">
-        <v>0.0385</v>
-      </c>
-      <c r="H56" t="n">
-        <v>10.5735</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
+      <c r="S56" t="n">
+        <v>0.9459</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0.1086</v>
+      </c>
+      <c r="U56" t="n">
         <v>1.2613</v>
       </c>
-      <c r="K56" t="n">
-        <v>3.6191</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0.1717</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
-        <v>0</v>
-      </c>
-      <c r="O56" t="n">
-        <v>0</v>
-      </c>
-      <c r="P56" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>0</v>
-      </c>
-      <c r="R56" t="n">
-        <v>0.9459</v>
-      </c>
-      <c r="S56" t="n">
+      <c r="V56" t="n">
         <v>0.049</v>
       </c>
-      <c r="T56" t="n">
+      <c r="W56" t="n">
         <v>0.0911</v>
-      </c>
-      <c r="U56" t="n">
-        <v>0.1086</v>
-      </c>
-      <c r="V56" t="n">
-        <v>3.0515</v>
-      </c>
-      <c r="W56" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4573,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -4597,7 +4597,7 @@
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>0.98</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
@@ -4646,64 +4646,64 @@
         <v>1</v>
       </c>
       <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="L58" t="n">
         <v>0.0036</v>
       </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="n">
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.1174</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="R58" t="n">
         <v>0.0036</v>
       </c>
-      <c r="G58" t="n">
-        <v>0.1174</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" t="n">
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0</v>
+      </c>
+      <c r="U58" t="n">
         <v>0.0587</v>
       </c>
-      <c r="K58" t="n">
-        <v>0.0053</v>
-      </c>
-      <c r="L58" t="n">
-        <v>0</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" t="n">
-        <v>0</v>
-      </c>
-      <c r="O58" t="n">
-        <v>0</v>
-      </c>
-      <c r="P58" t="n">
-        <v>0.0053</v>
-      </c>
-      <c r="Q58" t="n">
-        <v>0</v>
-      </c>
-      <c r="R58" t="n">
-        <v>0</v>
-      </c>
-      <c r="S58" t="n">
+      <c r="V58" t="n">
         <v>4.7884</v>
       </c>
-      <c r="T58" t="n">
+      <c r="W58" t="n">
         <v>0.0391</v>
-      </c>
-      <c r="U58" t="n">
-        <v>0</v>
-      </c>
-      <c r="V58" t="n">
-        <v>0.0338</v>
-      </c>
-      <c r="W58" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -4719,13 +4719,13 @@
         <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>0.1488</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>0.502</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -4743,7 +4743,7 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>0.1488</v>
+        <v>0</v>
       </c>
       <c r="M59" t="n">
         <v>0</v>
@@ -4758,13 +4758,13 @@
         <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>0.502</v>
+        <v>0</v>
       </c>
       <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
         <v>0.2975</v>
-      </c>
-      <c r="S59" t="n">
-        <v>0</v>
       </c>
       <c r="T59" t="n">
         <v>0</v>
@@ -4792,13 +4792,13 @@
         <v>2</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>0.9507</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>0.0218</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -4816,37 +4816,37 @@
         <v>0</v>
       </c>
       <c r="L60" t="n">
-        <v>0.9507</v>
+        <v>0</v>
       </c>
       <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
         <v>0.0044</v>
       </c>
-      <c r="N60" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" t="n">
-        <v>0</v>
-      </c>
-      <c r="P60" t="n">
-        <v>0</v>
-      </c>
       <c r="Q60" t="n">
-        <v>0.0218</v>
+        <v>0</v>
       </c>
       <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="n">
         <v>1.1426</v>
       </c>
-      <c r="S60" t="n">
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" t="n">
         <v>0.0131</v>
-      </c>
-      <c r="T60" t="n">
-        <v>0</v>
-      </c>
-      <c r="U60" t="n">
-        <v>0</v>
-      </c>
-      <c r="V60" t="n">
-        <v>0</v>
       </c>
       <c r="W60" t="n">
         <v>0</v>
@@ -4865,7 +4865,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>0.6935</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>0.6935</v>
+        <v>0</v>
       </c>
       <c r="M61" t="n">
         <v>0</v>
@@ -4907,10 +4907,10 @@
         <v>0</v>
       </c>
       <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="n">
         <v>1.1096</v>
-      </c>
-      <c r="S61" t="n">
-        <v>0</v>
       </c>
       <c r="T61" t="n">
         <v>0</v>
@@ -4938,7 +4938,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -4962,7 +4962,7 @@
         <v>0</v>
       </c>
       <c r="L62" t="n">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="M62" t="n">
         <v>0</v>
@@ -4980,10 +4980,10 @@
         <v>0</v>
       </c>
       <c r="R62" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="n">
         <v>7.76</v>
-      </c>
-      <c r="S62" t="n">
-        <v>0</v>
       </c>
       <c r="T62" t="n">
         <v>0</v>
@@ -5026,11 +5026,11 @@
         <v>0</v>
       </c>
       <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
         <v>0.5444</v>
       </c>
-      <c r="J63" t="n">
-        <v>0</v>
-      </c>
       <c r="K63" t="n">
         <v>0</v>
       </c>
@@ -5038,17 +5038,17 @@
         <v>0</v>
       </c>
       <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" t="n">
         <v>0.2722</v>
       </c>
-      <c r="N63" t="n">
-        <v>0</v>
-      </c>
-      <c r="O63" t="n">
-        <v>0</v>
-      </c>
-      <c r="P63" t="n">
-        <v>0</v>
-      </c>
       <c r="Q63" t="n">
         <v>0</v>
       </c>
@@ -5056,16 +5056,16 @@
         <v>0</v>
       </c>
       <c r="S63" t="n">
+        <v>0</v>
+      </c>
+      <c r="T63" t="n">
+        <v>0</v>
+      </c>
+      <c r="U63" t="n">
+        <v>0</v>
+      </c>
+      <c r="V63" t="n">
         <v>0.4355</v>
-      </c>
-      <c r="T63" t="n">
-        <v>0</v>
-      </c>
-      <c r="U63" t="n">
-        <v>0</v>
-      </c>
-      <c r="V63" t="n">
-        <v>0</v>
       </c>
       <c r="W63" t="n">
         <v>0</v>
@@ -5084,7 +5084,7 @@
         <v>2</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>2.63</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
@@ -5108,7 +5108,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>2.63</v>
+        <v>0</v>
       </c>
       <c r="M64" t="n">
         <v>0</v>
@@ -5126,10 +5126,10 @@
         <v>0</v>
       </c>
       <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="n">
         <v>2.18</v>
-      </c>
-      <c r="S64" t="n">
-        <v>0</v>
       </c>
       <c r="T64" t="n">
         <v>0</v>
@@ -5236,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>0.0688</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
@@ -5269,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>0.0688</v>
+        <v>0</v>
       </c>
       <c r="R66" t="n">
         <v>0</v>
@@ -5321,40 +5321,40 @@
         <v>0</v>
       </c>
       <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="T67" t="n">
+        <v>0</v>
+      </c>
+      <c r="U67" t="n">
         <v>5.11</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="n">
-        <v>0</v>
-      </c>
-      <c r="N67" t="n">
-        <v>0</v>
-      </c>
-      <c r="O67" t="n">
-        <v>0</v>
-      </c>
-      <c r="P67" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q67" t="n">
-        <v>0</v>
-      </c>
-      <c r="R67" t="n">
-        <v>5.23</v>
-      </c>
-      <c r="S67" t="n">
-        <v>0</v>
-      </c>
-      <c r="T67" t="n">
-        <v>0</v>
-      </c>
-      <c r="U67" t="n">
-        <v>0</v>
       </c>
       <c r="V67" t="n">
         <v>0</v>
@@ -5376,7 +5376,7 @@
         <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>3.0508</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -5400,7 +5400,7 @@
         <v>0</v>
       </c>
       <c r="L68" t="n">
-        <v>3.0508</v>
+        <v>0</v>
       </c>
       <c r="M68" t="n">
         <v>0</v>
@@ -5418,19 +5418,19 @@
         <v>0</v>
       </c>
       <c r="R68" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="n">
         <v>0.2183</v>
       </c>
-      <c r="S68" t="n">
+      <c r="T68" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" t="n">
         <v>0.3686</v>
-      </c>
-      <c r="T68" t="n">
-        <v>0</v>
-      </c>
-      <c r="U68" t="n">
-        <v>0</v>
-      </c>
-      <c r="V68" t="n">
-        <v>0</v>
       </c>
       <c r="W68" t="n">
         <v>0</v>
@@ -5467,40 +5467,40 @@
         <v>0</v>
       </c>
       <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0</v>
+      </c>
+      <c r="R69" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="n">
+        <v>0</v>
+      </c>
+      <c r="T69" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="U69" t="n">
         <v>1.25</v>
-      </c>
-      <c r="K69" t="n">
-        <v>0</v>
-      </c>
-      <c r="L69" t="n">
-        <v>0</v>
-      </c>
-      <c r="M69" t="n">
-        <v>0</v>
-      </c>
-      <c r="N69" t="n">
-        <v>0</v>
-      </c>
-      <c r="O69" t="n">
-        <v>0</v>
-      </c>
-      <c r="P69" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q69" t="n">
-        <v>0</v>
-      </c>
-      <c r="R69" t="n">
-        <v>0</v>
-      </c>
-      <c r="S69" t="n">
-        <v>0</v>
-      </c>
-      <c r="T69" t="n">
-        <v>0</v>
-      </c>
-      <c r="U69" t="n">
-        <v>2.3</v>
       </c>
       <c r="V69" t="n">
         <v>0</v>
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -5561,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="Q70" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="R70" t="n">
         <v>0</v>
@@ -5601,10 +5601,10 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>0.0506</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>0.1935</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -5625,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="n">
-        <v>0.1935</v>
+        <v>0</v>
       </c>
       <c r="O71" t="n">
         <v>0</v>
@@ -5634,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="Q71" t="n">
-        <v>0.0506</v>
+        <v>0</v>
       </c>
       <c r="R71" t="n">
         <v>0</v>

</xml_diff>